<commit_message>
ai auto add more pkg
</commit_message>
<xml_diff>
--- a/test/mysql.xlsx
+++ b/test/mysql.xlsx
@@ -96,8 +96,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyAlignment="false">
+      <alignment/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -392,62 +395,62 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="1" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>